<commit_message>
commit final report @nrdowling @ysh627
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -412,7 +412,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B2">
@@ -432,7 +432,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H2">
@@ -448,7 +448,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B3">
@@ -468,7 +468,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H3">
@@ -484,7 +484,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B4">
@@ -504,7 +504,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H4">
@@ -520,7 +520,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B5">
@@ -540,7 +540,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H5">
@@ -556,7 +556,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B6">
@@ -576,7 +576,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H6">
@@ -592,7 +592,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B7">
@@ -612,7 +612,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H7">
@@ -628,7 +628,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B8">
@@ -648,7 +648,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H8">
@@ -664,7 +664,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B9">
@@ -684,7 +684,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H9">
@@ -700,7 +700,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B10">
@@ -720,7 +720,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H10">
@@ -736,7 +736,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B11">
@@ -756,7 +756,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H11">
@@ -772,7 +772,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B12">
@@ -792,7 +792,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H12">
@@ -808,7 +808,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B13">
@@ -828,7 +828,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H13">
@@ -844,7 +844,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B14">
@@ -864,7 +864,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H14">
@@ -880,7 +880,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B15">
@@ -900,7 +900,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H15">
@@ -916,7 +916,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B16">
@@ -936,7 +936,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H16">
@@ -952,7 +952,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B17">
@@ -972,7 +972,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H17">
@@ -988,7 +988,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B18">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H18">
@@ -1024,7 +1024,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B19">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H19">
@@ -1060,7 +1060,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B20">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H20">
@@ -1096,7 +1096,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B21">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H21">
@@ -1132,7 +1132,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B22">
@@ -1152,7 +1152,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H22">
@@ -1168,7 +1168,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B23">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H23">
@@ -1204,7 +1204,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B24">
@@ -1224,7 +1224,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H24">
@@ -1240,7 +1240,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B25">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H25">
@@ -1276,7 +1276,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B26">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H26">
@@ -1312,7 +1312,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B27">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H27">
@@ -1348,7 +1348,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B28">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H28">
@@ -1384,7 +1384,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B29">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H29">
@@ -1420,7 +1420,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B30">
@@ -1440,7 +1440,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H30">
@@ -1456,7 +1456,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>higher-class</t>
+          <t>Higher-Class</t>
         </is>
       </c>
       <c r="B31">
@@ -1476,7 +1476,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H31">
@@ -1492,7 +1492,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B32">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H32">
@@ -1528,7 +1528,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B33">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H33">
@@ -1564,7 +1564,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B34">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H34">
@@ -1600,7 +1600,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B35">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H35">
@@ -1636,7 +1636,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B36">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H36">
@@ -1672,7 +1672,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B37">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H37">
@@ -1708,7 +1708,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B38">
@@ -1728,7 +1728,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H38">
@@ -1744,7 +1744,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B39">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H39">
@@ -1780,7 +1780,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B40">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H40">
@@ -1816,7 +1816,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B41">
@@ -1836,7 +1836,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H41">
@@ -1852,7 +1852,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B42">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H42">
@@ -1888,7 +1888,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B43">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H43">
@@ -1924,7 +1924,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B44">
@@ -1944,7 +1944,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H44">
@@ -1960,7 +1960,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B45">
@@ -1980,7 +1980,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H45">
@@ -1996,7 +1996,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B46">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H46">
@@ -2032,7 +2032,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B47">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H47">
@@ -2068,7 +2068,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B48">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H48">
@@ -2104,7 +2104,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B49">
@@ -2124,7 +2124,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H49">
@@ -2140,7 +2140,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B50">
@@ -2160,7 +2160,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H50">
@@ -2176,7 +2176,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B51">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H51">
@@ -2212,7 +2212,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B52">
@@ -2232,7 +2232,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H52">
@@ -2248,7 +2248,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B53">
@@ -2268,7 +2268,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H53">
@@ -2284,7 +2284,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B54">
@@ -2304,7 +2304,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H54">
@@ -2320,7 +2320,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B55">
@@ -2340,7 +2340,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H55">
@@ -2356,7 +2356,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B56">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H56">
@@ -2392,7 +2392,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B57">
@@ -2412,7 +2412,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H57">
@@ -2428,7 +2428,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B58">
@@ -2448,7 +2448,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H58">
@@ -2464,7 +2464,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B59">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H59">
@@ -2500,7 +2500,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B60">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H60">
@@ -2536,7 +2536,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B61">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H61">
@@ -2572,7 +2572,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B62">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H62">
@@ -2608,7 +2608,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B63">
@@ -2628,7 +2628,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H63">
@@ -2644,7 +2644,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B64">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H64">
@@ -2680,7 +2680,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B65">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H65">
@@ -2716,7 +2716,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B66">
@@ -2736,7 +2736,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="H66">
@@ -2752,7 +2752,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>lower-class</t>
+          <t>Lower-Class</t>
         </is>
       </c>
       <c r="B67">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="H67">

</xml_diff>